<commit_message>
Ejemplo est. Cond. Multiple
</commit_message>
<xml_diff>
--- a/Analisis de Problemas Algoritmicos.xlsx
+++ b/Analisis de Problemas Algoritmicos.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DAVIDMP 2021-2\FP\Sesion 04\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DAVIDMP 2021\CURSOS 2021-2\GU-Fundamentos de Programacion 2021-2\Sesion 05\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9120" windowHeight="8070" tabRatio="849" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16950" windowHeight="6990" tabRatio="849" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Est-Secuenciales-Ejer01" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="AREA-trapecio" sheetId="5" r:id="rId5"/>
     <sheet name="NOTA-promedio final" sheetId="6" r:id="rId6"/>
     <sheet name="G1-3.9" sheetId="7" r:id="rId7"/>
+    <sheet name="G1-T3.7" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -291,7 +292,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="135">
   <si>
     <t>Ponderación</t>
   </si>
@@ -887,6 +888,111 @@
         <scheme val="minor"/>
       </rPr>
       <t>min</t>
+    </r>
+  </si>
+  <si>
+    <t>Criterios:</t>
+  </si>
+  <si>
+    <t>Alumnos</t>
+  </si>
+  <si>
+    <t>edad&gt;18</t>
+  </si>
+  <si>
+    <t>Prom&gt;=9</t>
+  </si>
+  <si>
+    <t>$2000.00</t>
+  </si>
+  <si>
+    <t>$1000.00</t>
+  </si>
+  <si>
+    <t>Porm&lt;7.5 y Prom&gt;=6</t>
+  </si>
+  <si>
+    <t>$500.00</t>
+  </si>
+  <si>
+    <t>Prom&lt;6</t>
+  </si>
+  <si>
+    <t>Carta Estudien</t>
+  </si>
+  <si>
+    <t>edad&lt;=18</t>
+  </si>
+  <si>
+    <t>$3000.00</t>
+  </si>
+  <si>
+    <t>Prom&lt;9 y Prom&gt;=8</t>
+  </si>
+  <si>
+    <t>Prom&lt;8 y Prom&gt;=6</t>
+  </si>
+  <si>
+    <t>$100</t>
+  </si>
+  <si>
+    <t>Edad</t>
+  </si>
+  <si>
+    <t>Promedio</t>
+  </si>
+  <si>
+    <t>Beca</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>BC</t>
+  </si>
+  <si>
+    <t>NB</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>Simular</t>
+  </si>
+  <si>
+    <t>Monto $</t>
+  </si>
+  <si>
+    <t>Datos Entrada</t>
+  </si>
+  <si>
+    <t>Datos Salida</t>
+  </si>
+  <si>
+    <t>Mensual</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Prom&gt;=7.5 y </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Prom&lt;9</t>
     </r>
   </si>
 </sst>
@@ -1042,7 +1148,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1091,8 +1197,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1115,11 +1245,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1141,6 +1351,27 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1159,32 +1390,38 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1380,6 +1617,54 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>136071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect t="37650" b="2512"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="4429125" cy="2041071"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1665,20 +1950,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
     </row>
     <row r="2" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1755,11 +2040,11 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
       <c r="D8" s="6">
         <f>SUM(D4:D7)</f>
         <v>18.75</v>
@@ -1872,20 +2157,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -2007,11 +2292,11 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
       <c r="D11" s="13">
         <f>SUM(D4:D10)</f>
         <v>15.049999999999999</v>
@@ -2211,36 +2496,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
     </row>
     <row r="2" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="25"/>
+      <c r="C4" s="36"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -2393,12 +2678,12 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
       <c r="E13" s="20">
         <f>SUM(E6:E12)</f>
         <v>14.649999999999999</v>
@@ -2444,7 +2729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
@@ -2467,106 +2752,106 @@
   </cols>
   <sheetData>
     <row r="3" spans="9:18" x14ac:dyDescent="0.25">
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
     </row>
     <row r="4" spans="9:18" x14ac:dyDescent="0.25">
-      <c r="K4" s="27" t="s">
+      <c r="K4" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27" t="s">
+      <c r="L4" s="39"/>
+      <c r="M4" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27" t="s">
+      <c r="N4" s="39"/>
+      <c r="O4" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27" t="s">
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="R4" s="27"/>
+      <c r="R4" s="39"/>
     </row>
     <row r="5" spans="9:18" x14ac:dyDescent="0.25">
-      <c r="I5" s="31" t="s">
+      <c r="I5" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="K5" s="27" t="s">
+      <c r="K5" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27" t="s">
+      <c r="L5" s="39"/>
+      <c r="M5" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27" t="s">
+      <c r="N5" s="39"/>
+      <c r="O5" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="27" t="s">
+      <c r="P5" s="39"/>
+      <c r="Q5" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="R5" s="27"/>
-    </row>
-    <row r="6" spans="9:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="I6" s="31"/>
-      <c r="J6" s="39" t="s">
+      <c r="R5" s="39"/>
+    </row>
+    <row r="6" spans="9:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="I6" s="38"/>
+      <c r="J6" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="K6" s="28" t="s">
+      <c r="K6" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="L6" s="30">
+      <c r="L6" s="23">
         <v>1</v>
       </c>
-      <c r="M6" s="28" t="s">
+      <c r="M6" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="N6" s="30">
+      <c r="N6" s="23">
         <v>0.8</v>
       </c>
-      <c r="O6" s="28" t="s">
+      <c r="O6" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="P6" s="30">
+      <c r="P6" s="23">
         <v>0.7</v>
       </c>
-      <c r="Q6" s="28" t="s">
+      <c r="Q6" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="R6" s="30">
+      <c r="R6" s="23">
         <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="9:18" x14ac:dyDescent="0.25">
-      <c r="K9" s="27" t="s">
+      <c r="K9" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="L9" s="27"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27" t="s">
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="O9" s="27"/>
+      <c r="O9" s="39"/>
     </row>
     <row r="10" spans="9:18" x14ac:dyDescent="0.25">
-      <c r="I10" s="31" t="s">
+      <c r="I10" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="K10" s="29" t="s">
+      <c r="K10" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="L10" s="29" t="s">
+      <c r="L10" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="M10" s="29" t="s">
+      <c r="M10" s="22" t="s">
         <v>77</v>
       </c>
       <c r="N10" s="11" t="s">
@@ -2577,41 +2862,41 @@
       </c>
     </row>
     <row r="11" spans="9:18" x14ac:dyDescent="0.25">
-      <c r="I11" s="31"/>
-      <c r="K11" s="34">
+      <c r="I11" s="38"/>
+      <c r="K11" s="26">
         <v>0.03</v>
       </c>
-      <c r="L11" s="33">
+      <c r="L11" s="25">
         <v>0</v>
       </c>
-      <c r="M11" s="33">
+      <c r="M11" s="25">
         <v>0</v>
       </c>
-      <c r="N11" s="32">
+      <c r="N11" s="24">
         <v>0.15</v>
       </c>
-      <c r="O11" s="32">
+      <c r="O11" s="24">
         <v>0.1</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="16"/>
-      <c r="C25" s="38" t="s">
+      <c r="C25" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="D25" s="38" t="s">
+      <c r="D25" s="30" t="s">
         <v>78</v>
       </c>
       <c r="E25" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="F25" s="37" t="s">
+      <c r="F25" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="G25" s="37" t="s">
+      <c r="G25" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="H25" s="37" t="s">
+      <c r="H25" s="29" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2622,21 +2907,21 @@
       <c r="C26" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D26" s="36" t="s">
+      <c r="D26" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="E26" s="35">
+      <c r="E26" s="27">
         <v>5</v>
       </c>
-      <c r="F26" s="35">
+      <c r="F26" s="27">
         <f>(E26*$L$6)</f>
         <v>5</v>
       </c>
-      <c r="G26" s="35">
+      <c r="G26" s="27">
         <f>F26*0.15</f>
         <v>0.75</v>
       </c>
-      <c r="H26" s="35">
+      <c r="H26" s="27">
         <f>G26+F26</f>
         <v>5.75</v>
       </c>
@@ -2648,21 +2933,21 @@
       <c r="C27" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="D27" s="36" t="s">
+      <c r="D27" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="E27" s="35">
+      <c r="E27" s="27">
         <v>6</v>
       </c>
-      <c r="F27" s="35">
+      <c r="F27" s="27">
         <f>(5*1)+(1*0.8)</f>
         <v>5.8</v>
       </c>
-      <c r="G27" s="35">
+      <c r="G27" s="27">
         <f>F27*0.03</f>
         <v>0.17399999999999999</v>
       </c>
-      <c r="H27" s="35">
+      <c r="H27" s="27">
         <f>F27+G27</f>
         <v>5.9740000000000002</v>
       </c>
@@ -2674,21 +2959,21 @@
       <c r="C28" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D28" s="36" t="s">
+      <c r="D28" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="E28" s="35">
+      <c r="E28" s="27">
         <v>9</v>
       </c>
-      <c r="F28" s="35">
+      <c r="F28" s="27">
         <f>(5*1)+(3*0.8)+(1*0.7)</f>
         <v>8.1</v>
       </c>
-      <c r="G28" s="35">
+      <c r="G28" s="27">
         <f>F28*0.15</f>
         <v>1.2149999999999999</v>
       </c>
-      <c r="H28" s="35">
+      <c r="H28" s="27">
         <f>G28+F28</f>
         <v>9.3149999999999995</v>
       </c>
@@ -2700,40 +2985,268 @@
       <c r="C29" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D29" s="36" t="s">
+      <c r="D29" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="E29" s="35">
+      <c r="E29" s="27">
         <v>11</v>
       </c>
-      <c r="F29" s="35">
+      <c r="F29" s="27">
         <f>(5*1)+(3*0.8)+(2*0.7)+(1*0.5)</f>
         <v>9.3000000000000007</v>
       </c>
-      <c r="G29" s="35">
+      <c r="G29" s="27">
         <f>F29*0</f>
         <v>0</v>
       </c>
-      <c r="H29" s="35">
+      <c r="H29" s="27">
         <f>F29+G29</f>
         <v>9.3000000000000007</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="K3:P3"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q4:R4"/>
     <mergeCell ref="I10:I11"/>
     <mergeCell ref="K9:M9"/>
     <mergeCell ref="N9:O9"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="O4:P4"/>
-    <mergeCell ref="K3:P3"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
     <mergeCell ref="I5:I6"/>
-    <mergeCell ref="Q4:R4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E1:K17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" s="56" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="J2" s="57" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H3" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="I3" s="50" t="s">
+        <v>107</v>
+      </c>
+      <c r="J3" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="K3" s="51" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="H4" s="40"/>
+      <c r="I4" s="41" t="s">
+        <v>134</v>
+      </c>
+      <c r="J4" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="K4" s="42" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="H5" s="40"/>
+      <c r="I5" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="J5" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="K5" s="42" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="H6" s="40"/>
+      <c r="I6" s="58" t="s">
+        <v>112</v>
+      </c>
+      <c r="J6" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="K6" s="42" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="H7" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="I7" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="J7" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="K7" s="45" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="H8" s="43"/>
+      <c r="I8" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="J8" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="K8" s="45" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="H9" s="43"/>
+      <c r="I9" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="J9" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="K9" s="45" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="H10" s="46"/>
+      <c r="I10" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="J10" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="K10" s="48" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E12" s="53" t="s">
+        <v>131</v>
+      </c>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="54" t="s">
+        <v>132</v>
+      </c>
+      <c r="I12" s="54"/>
+    </row>
+    <row r="13" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="G13" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E14" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" s="59" t="s">
+        <v>119</v>
+      </c>
+      <c r="G14" s="59" t="s">
+        <v>120</v>
+      </c>
+      <c r="H14" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="I14" s="60" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E15" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F15" s="27">
+        <v>18</v>
+      </c>
+      <c r="G15" s="27">
+        <v>9</v>
+      </c>
+      <c r="H15" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="I15" s="27">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="16" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E16" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="27">
+        <v>20</v>
+      </c>
+      <c r="G16" s="27">
+        <v>8</v>
+      </c>
+      <c r="H16" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="I16" s="27">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E17" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" s="27">
+        <v>16</v>
+      </c>
+      <c r="G17" s="27">
+        <v>7</v>
+      </c>
+      <c r="H17" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="I17" s="27">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="H12:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>